<commit_message>
Move All Negative element to the one side of array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\DSA Supreme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\450 Dsa Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CB46D6-DE72-4643-8C10-1ADA8741C83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955BAA63-9897-445B-AA9C-B049D3687A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView minimized="1" xWindow="3375" yWindow="2925" windowWidth="15375" windowHeight="7875" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1423,6 +1423,12 @@
   </si>
   <si>
     <t>&lt;Yes&gt;</t>
+  </si>
+  <si>
+    <t>&lt;-Yes&gt;</t>
+  </si>
+  <si>
+    <t>&lt;-Yes-&gt;</t>
   </si>
 </sst>
 </file>
@@ -1868,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1916,26 +1922,26 @@
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="21">
-      <c r="A8" s="5" t="s">
+      <c r="C7" s="13" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>4</v>
+      <c r="C8" s="13" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="14" customFormat="1" ht="21">

</xml_diff>

<commit_message>
Union of two arrays
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\450 Dsa Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955BAA63-9897-445B-AA9C-B049D3687A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EA9014-CF58-41CC-9A9A-A4E34DBE3C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3375" yWindow="2925" windowWidth="15375" windowHeight="7875" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1875,7 +1875,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1955,37 +1955,37 @@
         <v>465</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21">
-      <c r="A11" s="5" t="s">
+      <c r="C10" s="13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="21">
-      <c r="A12" s="5" t="s">
+      <c r="C11" s="13" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>4</v>
+      <c r="C12" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Subarray with 0 sum
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\450 Dsa Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54D663E-0B11-4366-996C-4AD8282D5248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C6284A-BD0F-4C93-913E-7D94C8DDA57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1909,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2133,15 +2133,15 @@
         <v>465</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A23" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>4</v>
+      <c r="C23" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="14" customFormat="1" ht="21">
@@ -2166,15 +2166,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A26" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>4</v>
+      <c r="C26" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Factorials of large numbers
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\450 Dsa Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C6284A-BD0F-4C93-913E-7D94C8DDA57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E41F18-6A17-4DDB-9D75-2BEE5EEDABF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1910,7 +1910,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2155,48 +2155,48 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="14" customFormat="1" ht="21">
-      <c r="A26" s="11" t="s">
+      <c r="C25" s="13" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A26" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="17" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A27" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="21">
-      <c r="A28" s="5" t="s">
+      <c r="C27" s="17" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>4</v>
+      <c r="C28" s="17" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Median of 2 Sorted Arrays of Different Sizes
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\450 Dsa Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F588B4D-1CB6-4389-86E5-E77D1C6B0A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB92608C-ABD0-44CD-AA08-B0F94BF4CD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1498,7 +1498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1523,12 +1523,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1543,7 +1537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1591,14 +1585,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1923,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2345,14 +2331,14 @@
         <v>465</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="26" customFormat="1" ht="21">
-      <c r="A41" s="23" t="s">
+    <row r="41" spans="1:3" s="22" customFormat="1" ht="21">
+      <c r="A41" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="21" t="s">
         <v>465</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding 3 matrix problems
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\450 Dsa Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9622E22A-04EB-415D-9462-04573C6B0931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC6B132-F0D8-4F6C-B30D-849EACA155DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1537,7 +1537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1586,6 +1586,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1913,7 +1916,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2380,26 +2383,26 @@
         <v>465</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21">
-      <c r="A46" s="8" t="s">
+    <row r="46" spans="1:3" s="22" customFormat="1" ht="21">
+      <c r="A46" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="21">
-      <c r="A47" s="8" t="s">
+      <c r="C46" s="21" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="18" customFormat="1" ht="21">
+      <c r="A47" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>4</v>
+      <c r="C47" s="17" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Maximum difference between pair in a matrix
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\450 Dsa Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A1315E-DE91-4FE5-8E4A-C5CAE49A3717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8908649-B369-4041-8843-9BAE7644C6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1603,9 +1603,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFEAF468"/>
       <color rgb="FFF12B2B"/>
       <color rgb="FFCC0000"/>
+      <color rgb="FFEAF468"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1919,7 +1919,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2430,15 +2430,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21">
-      <c r="A50" s="8" t="s">
+    <row r="50" spans="1:3" s="22" customFormat="1" ht="21">
+      <c r="A50" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>4</v>
+      <c r="C50" s="21" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Remove all duplicates from a given string
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\450 Dsa Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1D6D02-34FC-47EA-B4B0-B3310CEA8950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B935F3-C9B2-4CFF-BB23-C2B783AAE9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1935,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2518,15 +2518,15 @@
         <v>465</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21">
-      <c r="A58" s="5" t="s">
+    <row r="58" spans="1:3" s="14" customFormat="1" ht="21">
+      <c r="A58" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>4</v>
+      <c r="C58" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="21">

</xml_diff>